<commit_message>
updated layout of input and output xlsx files
</commit_message>
<xml_diff>
--- a/etudiants.xlsx
+++ b/etudiants.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertr\Downloads\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertr\Documents\GitHub\labTeamCreator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6A052C-4E86-4EC0-B6C2-B8760C56820E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF40139C-69B7-4DF1-9A0B-DC8F4C8B8C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F97B6A08-D8A1-41B0-8A7D-6105B34B0937}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F97B6A08-D8A1-41B0-8A7D-6105B34B0937}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
-  <si>
-    <t>etudiants</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>b</t>
   </si>
@@ -74,13 +68,52 @@
     <t>egr</t>
   </si>
   <si>
-    <t>ge</t>
-  </si>
-  <si>
     <t>er</t>
   </si>
   <si>
     <t>lii</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>gg</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>ii</t>
+  </si>
+  <si>
+    <t>jj</t>
+  </si>
+  <si>
+    <t>dg</t>
+  </si>
+  <si>
+    <t>dfg</t>
   </si>
 </sst>
 </file>
@@ -432,97 +465,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A983D0C6-A590-4B9E-9468-39B81D65EABE}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>"a"</f>
+        <v>a</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
+      <c r="B16" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added full formatting of lab teams in teams.xlsx, using an excel template
and some bug fixes and other minor improvements
</commit_message>
<xml_diff>
--- a/etudiants.xlsx
+++ b/etudiants.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebby\Documents\GitHub\labTeamCreator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertr\Documents\GitHub\labTeamCreator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{392B5BDA-6219-481C-B2E4-11794C910AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8570D4F-EFE7-4B55-9361-92ABBBEFBE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="6435" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="gr.00020" sheetId="1" r:id="rId1"/>
-    <sheet name="gr.00021" sheetId="2" r:id="rId2"/>
+    <sheet name="gr.00021" sheetId="2" r:id="rId1"/>
+    <sheet name="gr.00020" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -879,16 +879,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E66B8BC-4980-4328-9A6A-DDA6E72D17A0}">
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -896,144 +896,174 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>"Bégin"</f>
-        <v>Bégin</v>
+        <f>"Cloutier"</f>
+        <v>Cloutier</v>
       </c>
       <c r="B2" t="str">
-        <f>"Alicia"</f>
-        <v>Alicia</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <f>"Annie"</f>
+        <v>Annie</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>"Bety"</f>
-        <v>Bety</v>
+        <f>"Couture"</f>
+        <v>Couture</v>
       </c>
       <c r="B3" t="str">
-        <f>"Jade"</f>
-        <v>Jade</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <f>"Samuel"</f>
+        <v>Samuel</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>"Boucher"</f>
-        <v>Boucher</v>
+        <f>"Doyon"</f>
+        <v>Doyon</v>
       </c>
       <c r="B4" t="str">
+        <f>"Clara"</f>
+        <v>Clara</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>"Doyon"</f>
+        <v>Doyon</v>
+      </c>
+      <c r="B5" t="str">
+        <f>"Yan Olivier"</f>
+        <v>Yan Olivier</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>"Fecteau"</f>
+        <v>Fecteau</v>
+      </c>
+      <c r="B6" t="str">
+        <f>"Amélie"</f>
+        <v>Amélie</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>"Gagné"</f>
+        <v>Gagné</v>
+      </c>
+      <c r="B7" t="str">
+        <f>"Élodie"</f>
+        <v>Élodie</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>"Labbé"</f>
+        <v>Labbé</v>
+      </c>
+      <c r="B8" t="str">
+        <f>"Éliana"</f>
+        <v>Éliana</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>"Latulippe"</f>
+        <v>Latulippe</v>
+      </c>
+      <c r="B9" t="str">
+        <f>"Laurence"</f>
+        <v>Laurence</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>"Lavergne"</f>
+        <v>Lavergne</v>
+      </c>
+      <c r="B10" t="str">
+        <f>"Ann-Sophie"</f>
+        <v>Ann-Sophie</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>"Lessard"</f>
+        <v>Lessard</v>
+      </c>
+      <c r="B11" t="str">
+        <f>"Émy"</f>
+        <v>Émy</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>"Marcoux"</f>
+        <v>Marcoux</v>
+      </c>
+      <c r="B12" t="str">
+        <f>"Kaylan"</f>
+        <v>Kaylan</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>"Méthot"</f>
+        <v>Méthot</v>
+      </c>
+      <c r="B13" t="str">
+        <f>"Alyssa"</f>
+        <v>Alyssa</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>"Nadeau"</f>
+        <v>Nadeau</v>
+      </c>
+      <c r="B14" t="str">
+        <f>"Myriam"</f>
+        <v>Myriam</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>"Pouliot"</f>
+        <v>Pouliot</v>
+      </c>
+      <c r="B15" t="str">
+        <f>"Justine"</f>
+        <v>Justine</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>"Rodrigue"</f>
+        <v>Rodrigue</v>
+      </c>
+      <c r="B16" t="str">
+        <f>"Aymrik"</f>
+        <v>Aymrik</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>"Roy"</f>
+        <v>Roy</v>
+      </c>
+      <c r="B17" t="str">
         <f>"Jeanne"</f>
         <v>Jeanne</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="str">
-        <f>"Chabot"</f>
-        <v>Chabot</v>
-      </c>
-      <c r="B5" t="str">
-        <f>"Amélie"</f>
-        <v>Amélie</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="str">
-        <f>"Couture"</f>
-        <v>Couture</v>
-      </c>
-      <c r="B6" t="str">
-        <f>"Marilou"</f>
-        <v>Marilou</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="str">
-        <f>"Drouin"</f>
-        <v>Drouin</v>
-      </c>
-      <c r="B7" t="str">
-        <f>"Emmy"</f>
-        <v>Emmy</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="str">
-        <f>"Gagné"</f>
-        <v>Gagné</v>
-      </c>
-      <c r="B8" t="str">
-        <f>"Claudia"</f>
-        <v>Claudia</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="str">
-        <f>"Giroux"</f>
-        <v>Giroux</v>
-      </c>
-      <c r="B9" t="str">
-        <f>"Mélodie"</f>
-        <v>Mélodie</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="str">
-        <f>"Guay"</f>
-        <v>Guay</v>
-      </c>
-      <c r="B10" t="str">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>"Vallières"</f>
+        <v>Vallières</v>
+      </c>
+      <c r="B18" t="str">
         <f>"Anne-Marie"</f>
         <v>Anne-Marie</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="str">
-        <f>"Jacques"</f>
-        <v>Jacques</v>
-      </c>
-      <c r="B11" t="str">
-        <f>"Rosalie"</f>
-        <v>Rosalie</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="str">
-        <f>"Paradis"</f>
-        <v>Paradis</v>
-      </c>
-      <c r="B12" t="str">
-        <f>"Jessica"</f>
-        <v>Jessica</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="str">
-        <f>"Paradis"</f>
-        <v>Paradis</v>
-      </c>
-      <c r="B13" t="str">
-        <f>"Mégane"</f>
-        <v>Mégane</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="str">
-        <f>"Roy"</f>
-        <v>Roy</v>
-      </c>
-      <c r="B14" t="str">
-        <f>"Justine"</f>
-        <v>Justine</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="str">
-        <f>"Vaillancourt"</f>
-        <v>Vaillancourt</v>
-      </c>
-      <c r="B15" t="str">
-        <f>"Kelly"</f>
-        <v>Kelly</v>
       </c>
     </row>
   </sheetData>
@@ -1042,16 +1072,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E66B8BC-4980-4328-9A6A-DDA6E72D17A0}">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1059,174 +1089,144 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>"Cloutier"</f>
-        <v>Cloutier</v>
+        <f>"Bégin"</f>
+        <v>Bégin</v>
       </c>
       <c r="B2" t="str">
-        <f>"Annie"</f>
-        <v>Annie</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <f>"Alicia"</f>
+        <v>Alicia</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
+        <f>"Bety"</f>
+        <v>Bety</v>
+      </c>
+      <c r="B3" t="str">
+        <f>"Jade"</f>
+        <v>Jade</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>"Boucher"</f>
+        <v>Boucher</v>
+      </c>
+      <c r="B4" t="str">
+        <f>"Jeanne"</f>
+        <v>Jeanne</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>"Chabot"</f>
+        <v>Chabot</v>
+      </c>
+      <c r="B5" t="str">
+        <f>"Amélie"</f>
+        <v>Amélie</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
         <f>"Couture"</f>
         <v>Couture</v>
       </c>
-      <c r="B3" t="str">
-        <f>"Samuel"</f>
-        <v>Samuel</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="str">
-        <f>"Doyon"</f>
-        <v>Doyon</v>
-      </c>
-      <c r="B4" t="str">
-        <f>"Clara"</f>
-        <v>Clara</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="str">
-        <f>"Doyon"</f>
-        <v>Doyon</v>
-      </c>
-      <c r="B5" t="str">
-        <f>"Yan Olivier"</f>
-        <v>Yan Olivier</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="str">
-        <f>"Fecteau"</f>
-        <v>Fecteau</v>
-      </c>
       <c r="B6" t="str">
-        <f>"Amélie"</f>
-        <v>Amélie</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <f>"Marilou"</f>
+        <v>Marilou</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
+        <f>"Drouin"</f>
+        <v>Drouin</v>
+      </c>
+      <c r="B7" t="str">
+        <f>"Emmy"</f>
+        <v>Emmy</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
         <f>"Gagné"</f>
         <v>Gagné</v>
       </c>
-      <c r="B7" t="str">
-        <f>"Élodie"</f>
-        <v>Élodie</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="str">
-        <f>"Labbé"</f>
-        <v>Labbé</v>
-      </c>
       <c r="B8" t="str">
-        <f>"Éliana"</f>
-        <v>Éliana</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <f>"Claudia"</f>
+        <v>Claudia</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>"Latulippe"</f>
-        <v>Latulippe</v>
+        <f>"Giroux"</f>
+        <v>Giroux</v>
       </c>
       <c r="B9" t="str">
-        <f>"Laurence"</f>
-        <v>Laurence</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <f>"Mélodie"</f>
+        <v>Mélodie</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>"Lavergne"</f>
-        <v>Lavergne</v>
+        <f>"Guay"</f>
+        <v>Guay</v>
       </c>
       <c r="B10" t="str">
-        <f>"Ann-Sophie"</f>
-        <v>Ann-Sophie</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <f>"Anne-Marie"</f>
+        <v>Anne-Marie</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>"Lessard"</f>
-        <v>Lessard</v>
+        <f>"Jacques"</f>
+        <v>Jacques</v>
       </c>
       <c r="B11" t="str">
-        <f>"Émy"</f>
-        <v>Émy</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <f>"Rosalie"</f>
+        <v>Rosalie</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>"Marcoux"</f>
-        <v>Marcoux</v>
+        <f>"Paradis"</f>
+        <v>Paradis</v>
       </c>
       <c r="B12" t="str">
-        <f>"Kaylan"</f>
-        <v>Kaylan</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <f>"Jessica"</f>
+        <v>Jessica</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>"Méthot"</f>
-        <v>Méthot</v>
+        <f>"Paradis"</f>
+        <v>Paradis</v>
       </c>
       <c r="B13" t="str">
-        <f>"Alyssa"</f>
-        <v>Alyssa</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <f>"Mégane"</f>
+        <v>Mégane</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>"Nadeau"</f>
-        <v>Nadeau</v>
+        <f>"Roy"</f>
+        <v>Roy</v>
       </c>
       <c r="B14" t="str">
-        <f>"Myriam"</f>
-        <v>Myriam</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="str">
-        <f>"Pouliot"</f>
-        <v>Pouliot</v>
-      </c>
-      <c r="B15" t="str">
         <f>"Justine"</f>
         <v>Justine</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="str">
-        <f>"Rodrigue"</f>
-        <v>Rodrigue</v>
-      </c>
-      <c r="B16" t="str">
-        <f>"Aymrik"</f>
-        <v>Aymrik</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="str">
-        <f>"Roy"</f>
-        <v>Roy</v>
-      </c>
-      <c r="B17" t="str">
-        <f>"Jeanne"</f>
-        <v>Jeanne</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="str">
-        <f>"Vallières"</f>
-        <v>Vallières</v>
-      </c>
-      <c r="B18" t="str">
-        <f>"Anne-Marie"</f>
-        <v>Anne-Marie</v>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>"Vaillancourt"</f>
+        <v>Vaillancourt</v>
+      </c>
+      <c r="B15" t="str">
+        <f>"Kelly"</f>
+        <v>Kelly</v>
       </c>
     </row>
   </sheetData>

</xml_diff>